<commit_message>
Updated File--Added Regression.xml file
</commit_message>
<xml_diff>
--- a/src/main/java/com/nopcommerce/qa/TestData/nop_Commerce.xlsx
+++ b/src/main/java/com/nopcommerce/qa/TestData/nop_Commerce.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/51b133f81c7e6ee9/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="14_{DB2AB839-BD63-452B-A399-C6E2DA61DBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0696F345-2CCC-49CD-83C2-576DC11D739F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1076D70C-5781-45DE-9EE0-FFEBF4A302E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1BA27602-E22E-47CB-AE59-641E23A8C088}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="23280" windowHeight="13224" xr2:uid="{1BA27602-E22E-47CB-AE59-641E23A8C088}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>FirstName</t>
   </si>
@@ -42,9 +38,6 @@
     <t>DOB-Year</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>CompanyName</t>
   </si>
   <si>
@@ -72,9 +65,6 @@
     <t>March</t>
   </si>
   <si>
-    <t>umesh.singh@gmail.com</t>
-  </si>
-  <si>
     <t>ForceTechMah</t>
   </si>
   <si>
@@ -87,9 +77,6 @@
     <t>July</t>
   </si>
   <si>
-    <t>Ganesh.singh@gmail.com</t>
-  </si>
-  <si>
     <t>TechFutureMec</t>
   </si>
   <si>
@@ -102,9 +89,6 @@
     <t>August</t>
   </si>
   <si>
-    <t>Naveen.Singh@gmai.com</t>
-  </si>
-  <si>
     <t>GooglerTech</t>
   </si>
   <si>
@@ -121,9 +105,6 @@
   </si>
   <si>
     <t>Female</t>
-  </si>
-  <si>
-    <t>knwrpl345676@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -511,7 +492,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J5"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,15 +503,14 @@
     <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -554,156 +534,137 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2">
         <v>1990</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2">
         <v>1995</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="I3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
         <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="2">
         <v>2000</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>21</v>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
         <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2">
         <v>2005</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>26</v>
+      <c r="G5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{76ABEAFC-8FFC-433E-9A7C-EFE5B3C81075}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{5D28C6BB-E535-44FD-9AB4-1941F929EECA}"/>
-    <hyperlink ref="G2" r:id="rId3" xr:uid="{D6122615-B7AC-47A8-9499-67EA92ED46B2}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{265ACE3A-7B3E-429F-8F5A-D490590E9570}"/>
-    <hyperlink ref="G4" r:id="rId5" xr:uid="{9D0F43C4-0CB7-4CC2-9716-13BF3987F6CB}"/>
-    <hyperlink ref="I4" r:id="rId6" xr:uid="{329DE6AA-7DBC-49B1-BFB5-912BDF57CB2A}"/>
-    <hyperlink ref="G5" r:id="rId7" xr:uid="{3B492293-E126-4435-A4E8-98821BAAE71F}"/>
-    <hyperlink ref="I5" r:id="rId8" xr:uid="{0EB79FD6-D6F6-4048-B1E1-6D846E7407CB}"/>
-    <hyperlink ref="J2" r:id="rId9" xr:uid="{DA32DB8A-04B9-4FF1-ABBA-866502D6B1B5}"/>
-    <hyperlink ref="J3" r:id="rId10" xr:uid="{D72ABE47-7E66-4749-B1C3-533977ECDE93}"/>
-    <hyperlink ref="J4" r:id="rId11" xr:uid="{23703329-68BC-4609-9A2A-160BC1E2C446}"/>
-    <hyperlink ref="J5" r:id="rId12" xr:uid="{108F1042-345F-4C1B-9180-7FCF4F0DDD38}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{76ABEAFC-8FFC-433E-9A7C-EFE5B3C81075}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{265ACE3A-7B3E-429F-8F5A-D490590E9570}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{329DE6AA-7DBC-49B1-BFB5-912BDF57CB2A}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{0EB79FD6-D6F6-4048-B1E1-6D846E7407CB}"/>
+    <hyperlink ref="I2" r:id="rId5" xr:uid="{DA32DB8A-04B9-4FF1-ABBA-866502D6B1B5}"/>
+    <hyperlink ref="I3" r:id="rId6" xr:uid="{D72ABE47-7E66-4749-B1C3-533977ECDE93}"/>
+    <hyperlink ref="I4" r:id="rId7" xr:uid="{23703329-68BC-4609-9A2A-160BC1E2C446}"/>
+    <hyperlink ref="I5" r:id="rId8" xr:uid="{108F1042-345F-4C1B-9180-7FCF4F0DDD38}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>